<commit_message>
updated flask app to include all params
</commit_message>
<xml_diff>
--- a/Data/API_data_dictionary.xlsx
+++ b/Data/API_data_dictionary.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjaminpollock/Desktop/Project_2/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22C48114-97C5-AB48-AE29-5E818BE88657}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52752BBD-E96F-2D47-AD3A-0640D7CB8820}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33460" yWindow="1460" windowWidth="27640" windowHeight="16080" xr2:uid="{144FF619-4A8A-644D-813A-EE808C447428}"/>
+    <workbookView xWindow="3020" yWindow="460" windowWidth="22760" windowHeight="16620" activeTab="2" xr2:uid="{144FF619-4A8A-644D-813A-EE808C447428}"/>
   </bookViews>
   <sheets>
     <sheet name="States" sheetId="2" r:id="rId1"/>
     <sheet name="Causes" sheetId="1" r:id="rId2"/>
+    <sheet name="Dates" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="109">
   <si>
     <t>cause3</t>
   </si>
@@ -352,6 +353,15 @@
   </si>
   <si>
     <t>States</t>
+  </si>
+  <si>
+    <t>Max Date</t>
+  </si>
+  <si>
+    <t>Min Date</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
@@ -416,10 +426,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -736,8 +747,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4049F78-8571-FC48-87B0-44C475D7C6EB}">
   <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1007,343 +1018,638 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{829A4174-4C3C-AD44-AA07-F57C0BF4BABF}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:H34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H1" s="2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="1">
+        <v>20010</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1">
+        <v>529</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" s="1">
+        <v>60</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H2" s="1">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="1">
+        <v>3945</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1">
+        <v>251</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="F3" s="1">
+        <v>110</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H3" s="1">
+        <v>1721</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="1">
+        <v>5647</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1">
+        <v>1500</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F4" s="1">
+        <v>8</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H4" s="1">
+        <v>25668</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1">
+        <v>2520</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="F5" s="1">
+        <v>8</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="H5" s="1">
+        <v>892</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1">
+        <v>2163</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F6" s="1">
+        <v>44</v>
+      </c>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="1"/>
+      <c r="C7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1">
+        <v>8</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F7" s="1">
+        <v>203</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="1"/>
+      <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1">
+        <v>6351</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F8" s="1">
+        <v>80</v>
+      </c>
+      <c r="G8" s="1"/>
+      <c r="H8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="1"/>
+      <c r="C9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1">
+        <v>2188</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F9" s="1">
+        <v>892</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1">
+        <v>2901</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F10" s="1">
+        <v>3</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
+      <c r="B11" s="1"/>
+      <c r="C11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1">
+        <v>3543</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F11" s="1">
+        <v>34</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="D12" s="1">
+        <v>7353</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F12" s="1">
+        <v>166</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="1"/>
+      <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1">
+        <v>83</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F13" s="1">
+        <v>1001</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1">
+        <v>199</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F14" s="1">
+        <v>1321</v>
+      </c>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1">
+        <v>7</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F15" s="1">
+        <v>94</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="1"/>
+      <c r="C16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1">
+        <v>4</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F16" s="1">
+        <v>926</v>
+      </c>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="D17" s="1">
+        <v>2</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F17" s="1">
+        <v>6</v>
+      </c>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
-      <c r="C18" s="1" t="s">
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F18" s="1">
+        <v>83</v>
+      </c>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F19" s="1">
+        <v>1</v>
+      </c>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F20" s="1">
+        <v>214</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F21" s="1">
+        <v>409</v>
+      </c>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
-      <c r="C22" s="1" t="s">
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F22" s="1">
+        <v>60</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F23" s="1">
+        <v>18329</v>
+      </c>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F24" s="1">
+        <v>309</v>
+      </c>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F25" s="1">
+        <v>217</v>
+      </c>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F26" s="1">
+        <v>1880</v>
+      </c>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F27" s="1">
+        <v>24</v>
+      </c>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F28" s="1">
+        <v>36</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F29" s="1">
+        <v>23</v>
+      </c>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F30" s="1">
+        <v>484</v>
+      </c>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F31" s="1">
+        <v>199</v>
+      </c>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F32" s="1">
+        <v>2</v>
+      </c>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="F33" s="1">
+        <v>1314</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
-      <c r="C34" s="1" t="s">
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D34" s="1"/>
+      <c r="F34" s="1">
+        <v>1062</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{562EC6B9-369F-0645-9A5A-83E529317CFB}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>41275</v>
+      </c>
+      <c r="B2" s="3">
+        <v>42925</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>